<commit_message>
made modifications to the html converter to avoid leaving nan values in 'Year' column
</commit_message>
<xml_diff>
--- a/src/data/plan.xlsx
+++ b/src/data/plan.xlsx
@@ -2321,7 +2321,11 @@
           <t>GIINFOP1</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr"/>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="inlineStr">
         <is>
@@ -2353,7 +2357,11 @@
           <t>GIINFSNEG</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr"/>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
@@ -2385,7 +2393,11 @@
           <t>GIINFDPOI</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr"/>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
@@ -2409,7 +2421,11 @@
           <t>GIINFCD</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr"/>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
@@ -2433,7 +2449,11 @@
           <t>GIINFDAO</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr"/>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
@@ -2457,7 +2477,11 @@
           <t>GIINFSEGI2</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr"/>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
@@ -2481,7 +2505,11 @@
           <t>GIINFSISINTN</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr"/>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
@@ -2505,7 +2533,11 @@
           <t>GIINFSISTD2</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr"/>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
@@ -2529,7 +2561,11 @@
           <t>GIINFADDAT</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr"/>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E62" t="inlineStr"/>
       <c r="F62" t="inlineStr">
         <is>
@@ -2553,7 +2589,11 @@
           <t>GIINFBIDAT</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr"/>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E63" t="inlineStr"/>
       <c r="F63" t="inlineStr">
         <is>
@@ -2577,7 +2617,11 @@
           <t>GIINFCOMPG00</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E64" t="inlineStr"/>
       <c r="F64" t="inlineStr">
         <is>
@@ -2601,7 +2645,11 @@
           <t>GIINFDSDIG</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr"/>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E65" t="inlineStr"/>
       <c r="F65" t="inlineStr">
         <is>
@@ -2625,7 +2673,11 @@
           <t>GIINFEMTEC</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E66" t="inlineStr"/>
       <c r="F66" t="inlineStr">
         <is>
@@ -2649,7 +2701,11 @@
           <t>GIINFISOF</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E67" t="inlineStr"/>
       <c r="F67" t="inlineStr">
         <is>
@@ -2673,7 +2729,11 @@
           <t>GIINFRVIRT</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E68" t="inlineStr"/>
       <c r="F68" t="inlineStr">
         <is>
@@ -2697,7 +2757,11 @@
           <t>GIINDAUTOMT</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E69" t="inlineStr"/>
       <c r="F69" t="inlineStr">
         <is>
@@ -2721,7 +2785,11 @@
           <t>GIINFINTEC</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E70" t="inlineStr"/>
       <c r="F70" t="inlineStr">
         <is>
@@ -2745,7 +2813,11 @@
           <t>GIINFRVA</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr"/>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E71" t="inlineStr"/>
       <c r="F71" t="inlineStr">
         <is>
@@ -2769,7 +2841,11 @@
           <t>GIINDSSOPDEC</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr"/>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E72" t="inlineStr"/>
       <c r="F72" t="inlineStr">
         <is>
@@ -2793,7 +2869,11 @@
           <t>GIINFSCOM</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr"/>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E73" t="inlineStr"/>
       <c r="F73" t="inlineStr">
         <is>
@@ -2817,7 +2897,11 @@
           <t>GIINFSISTEXP</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr"/>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E74" t="inlineStr"/>
       <c r="F74" t="inlineStr">
         <is>
@@ -2841,7 +2925,11 @@
           <t>GIINFOP3</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr"/>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E75" t="inlineStr"/>
       <c r="F75" t="inlineStr">
         <is>
@@ -2865,7 +2953,11 @@
           <t>GIINFTP</t>
         </is>
       </c>
-      <c r="D76" t="inlineStr"/>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E76" t="inlineStr"/>
       <c r="F76" t="inlineStr">
         <is>
@@ -2889,7 +2981,11 @@
           <t>GIINDFISIII</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr"/>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E77" t="inlineStr"/>
       <c r="F77" t="inlineStr">
         <is>
@@ -2913,7 +3009,11 @@
           <t>GIINFLOG</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr"/>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E78" t="inlineStr"/>
       <c r="F78" t="inlineStr">
         <is>
@@ -2937,7 +3037,11 @@
           <t>GIINFMRR</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr"/>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E79" t="inlineStr"/>
       <c r="F79" t="inlineStr">
         <is>
@@ -2961,7 +3065,11 @@
           <t>GIINDQUI1</t>
         </is>
       </c>
-      <c r="D80" t="inlineStr"/>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E80" t="inlineStr"/>
       <c r="F80" t="inlineStr">
         <is>
@@ -2985,7 +3093,11 @@
           <t>GIINDSISINF</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr"/>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E81" t="inlineStr"/>
       <c r="F81" t="inlineStr">
         <is>
@@ -3009,7 +3121,11 @@
           <t>GIINFCBSEMB</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr"/>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E82" t="inlineStr"/>
       <c r="F82" t="inlineStr">
         <is>
@@ -3033,7 +3149,11 @@
           <t>GIINFINTROIA</t>
         </is>
       </c>
-      <c r="D83" t="inlineStr"/>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Electives</t>
+        </is>
+      </c>
       <c r="E83" t="inlineStr"/>
       <c r="F83" t="inlineStr">
         <is>
@@ -3057,7 +3177,11 @@
           <t>GIINFPRA.PROF</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr"/>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Other Requirements</t>
+        </is>
+      </c>
       <c r="E84" t="inlineStr"/>
       <c r="F84" t="inlineStr">
         <is>
@@ -3089,7 +3213,11 @@
           <t>GFIEXTVU</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr"/>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Other Requirements</t>
+        </is>
+      </c>
       <c r="E85" t="inlineStr"/>
       <c r="F85" t="inlineStr">
         <is>
@@ -3113,7 +3241,11 @@
           <t>GIINFTEOE</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr"/>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Other Requirements</t>
+        </is>
+      </c>
       <c r="E86" t="inlineStr"/>
       <c r="F86" t="inlineStr">
         <is>
@@ -3137,7 +3269,11 @@
           <t>GEXTING</t>
         </is>
       </c>
-      <c r="D87" t="inlineStr"/>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Other Requirements</t>
+        </is>
+      </c>
       <c r="E87" t="inlineStr"/>
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
@@ -3157,7 +3293,11 @@
           <t>GEXTILEV2</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr"/>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Other Requirements</t>
+        </is>
+      </c>
       <c r="E88" t="inlineStr"/>
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
@@ -3177,7 +3317,11 @@
           <t>GIINFSCP</t>
         </is>
       </c>
-      <c r="D89" t="inlineStr"/>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Other Requirements</t>
+        </is>
+      </c>
       <c r="E89" t="inlineStr"/>
       <c r="F89" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fixed minor issue with Node, updated python code and added new json file
</commit_message>
<xml_diff>
--- a/src/data/plan.xlsx
+++ b/src/data/plan.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,11 +434,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>index</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Course</t>
@@ -472,6 +467,16 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Prerequisites to Pass</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>is Prerequisite to Take of</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>is Prerequisite to Pass of</t>
         </is>
       </c>
     </row>
@@ -502,10 +507,20 @@
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>(GIINDAM2, Regularizada), (GIINDFIS1, Regularizada), (GIINDAM3, Aprobada), (GIINFAM4, Aprobada), (GIINDEST1, Regularizada), (GIINDEST2, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>(GIINDAM2, Aprobada), (GIINDFIS1, Aprobada), (GIINDEST1, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -530,10 +545,20 @@
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>(GIINDAL2, Regularizada), (GIINFAL3, Aprobada), (GIINFMD, Aprobada), (GIINDIOP, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>(GIINDAL2, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -558,10 +583,20 @@
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>(GIINFIP2, Regularizada), (GIINFLCD, Regularizada), (GIINFOC, Aprobada), (GIINFAED, Aprobada), (GIINFTE, Aprobada), (GIINFRCDA, Aprobada), (GIINFICO, Aprobada), (GIINFDIN, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>(GIINFIP2, Aprobada), (GIINFLCD, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -586,10 +621,20 @@
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>(GIINFTE, Regularizada), (GIINDTECOM, Aprobada), (GIINDLEG, Aprobada), (GIINDCON.Y PRE, Aprobada), (GIINDFHUM, Aprobada), (GIINDECON.POL, Aprobada), (GIINFOP1, Aprobada), (GIINFSNEG, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>(GIINFTE, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -614,10 +659,20 @@
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>(GIINDTE1, Regularizada), (GIINDANTROP, Regularizada), (GIINDETGEN, Aprobada), (GIINDTE2, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>(GIINDTE1, Aprobada), (GIINDANTROP, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -650,10 +705,20 @@
           <t>(GIINDAM1, Aprobada)</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>(GIINDAM3, Regularizada), (GIINFAM4, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>(GIINDAM3, Aprobada), (GIINFAM4, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -686,10 +751,20 @@
           <t>(GIINDAL1, Aprobada)</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>(GIINFAL3, Regularizada), (GIINFMD, Regularizada), (GIINDIOP, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>(GIINFAL3, Aprobada), (GIINFMD, Aprobada), (GIINDIOP, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -722,10 +797,20 @@
           <t>(GIINFPR1, Aprobada)</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>(GIINFAED, Regularizada), (GIINFADA, Aprobada), (GIINFBD, Aprobada), (GIINFTE, Regularizada), (GIINFL1, Aprobada), (GIINFICO, Regularizada), (GIINFDIN, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>(GIINFAED, Aprobada), (GIINFTE, Aprobada), (GIINFICO, Aprobada), (GIINFDIN, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -758,10 +843,20 @@
           <t>(GIINDAM1, Aprobada)</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>(GIINDEYM, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>(GIINDEYM, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -794,10 +889,20 @@
           <t>(GIINFPR1, Aprobada)</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>(GIINFSISOP, Aprobada), (GIINFICO, Regularizada), (GIINFSEGI, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>(GIINFOC, Aprobada), (GIINFRCDA, Aprobada), (GIINFICO, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -830,10 +935,20 @@
           <t>(GIINFLCD, Aprobada)</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>(GIINFSISOP, Regularizada), (GIINFPC, Aprobada), (GIINFSEGI, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>(GIINFSISOP, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -866,10 +981,12 @@
           <t>(GIINDAM2, Aprobada)</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -902,10 +1019,12 @@
           <t>(GIINDAL2, Aprobada)</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -938,10 +1057,12 @@
           <t>(GIINDFIS1, Aprobada)</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -974,10 +1095,20 @@
           <t>(GIINFIP2, Aprobada)</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>(GIINFADA, Regularizada), (GIINFBD, Regularizada), (GIINFL1, Regularizada), (GIINFDS, Aprobada), (GIINFL2, Aprobada), (GIINFLP, Aprobada), (GIINFOPMLINF, Aprobada), (GIINFSISTD1, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>(GIINFADA, Aprobada), (GIINFBD, Aprobada), (GIINFL1, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1010,10 +1141,20 @@
           <t>(GIINDIFI, Aprobada)</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>(GIINDTE2, Regularizada), (GIINDDOSIG, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>(GIINDTE2, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1046,10 +1187,12 @@
           <t>(GIINDAM2, Aprobada)</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1080,12 +1223,22 @@
       <c r="H19" t="inlineStr">
         <is>
           <t>(GIINDAM1, Aprobada)</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>(GIINDEST2, Regularizada), (GIINDIOP, Aprobada), (GIINFOPMLINF, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>(GIINDEST2, Aprobada)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1118,10 +1271,12 @@
           <t>(GIINDAL2, Aprobada)</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1152,12 +1307,22 @@
       <c r="H21" t="inlineStr">
         <is>
           <t>(GIINFAED, Aprobada)</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>(GIINFDS, Regularizada), (GIINFINGS, Aprobada), (GIINFLP, Regularizada), (GIINFL3, Aprobada), (GIINFPC, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>(GIINFDS, Aprobada), (GIINFLP, Aprobada)</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1188,12 +1353,22 @@
       <c r="H22" t="inlineStr">
         <is>
           <t>(GIINDIFI, Aprobada)</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>(GIINDETGEN, Regularizada), (GIINDETPROF, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>(GIINDETGEN, Aprobada)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1224,12 +1399,22 @@
       <c r="H23" t="inlineStr">
         <is>
           <t>(GIINFOC, Aprobada)</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>(GIINFPC, Regularizada), (GIINFSEGI, Regularizada), (GIINFSISTD1, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>(GIINFPC, Aprobada), (GIINFSEGI, Aprobada)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>79</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1260,12 +1445,22 @@
       <c r="H24" t="inlineStr">
         <is>
           <t>(GIINFAED, Aprobada)</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>(GIINFDS, Regularizada), (GIINFOPMLINF, Regularizada), (GIINFSISTD1, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>(GIINFDS, Aprobada), (GIINFOPMLINF, Aprobada), (GIINFSISTD1, Aprobada)</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1298,10 +1493,20 @@
           <t>(GIINDINING, Aprobada), (GIINFIP2, Aprobada)</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>(GIINDTECOM, Regularizada), (GIINDLEG, Regularizada), (GIINDCON.Y PRE, Regularizada), (GIINDFHUM, Regularizada), (GIINDECON.POL, Regularizada), (GIINFOP1, Regularizada), (GIINFSNEG, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>(GIINDTECOM, Aprobada), (GIINDLEG, Aprobada), (GIINDCON.Y PRE, Aprobada), (GIINDFHUM, Aprobada), (GIINDECON.POL, Aprobada), (GIINFOP1, Aprobada), (GIINFSNEG, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1334,10 +1539,20 @@
           <t>(GIINDEST1, Aprobada)</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>(GIINDIOP, Regularizada), (GIINFOPMLINF, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>(GIINDIOP, Aprobada), (GIINFOPMLINF, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1370,10 +1585,20 @@
           <t>(GIINFAED, Aprobada)</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>(GIINFL2, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>(GIINFL2, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1406,10 +1631,20 @@
           <t>(GIINFLCD, Aprobada)</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>(GIINFSEGI, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>(GIINFSEGI, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1442,10 +1677,12 @@
           <t>(GIINFLCD, Aprobada), (GIINFIP2, Aprobada)</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1478,10 +1715,20 @@
           <t>(GIINDANTROP, Aprobada)</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>(GIINDETPROF, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>(GIINDETPROF, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -1514,10 +1761,20 @@
           <t>(GIINFADA, Aprobada), (GIINFBD, Aprobada)</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>(GIINFINGS, Regularizada), (GIINFL3, Regularizada), (GIINFASCS, Aprobada), (GIINFDDP, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>(GIINFINGS, Aprobada), (GIINFL3, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1550,10 +1807,12 @@
           <t>(GIINFL1, Aprobada)</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1586,10 +1845,20 @@
           <t>(GIINFDS, Aprobada)</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>(GIINFASCS, Regularizada), (GIINFDDP, Regularizada), (GIINFL4, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>(GIINFASCS, Aprobada), (GIINFDDP, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -1622,10 +1891,20 @@
           <t>(GIINFADA, Aprobada)</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>(GIINFPC, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>(GIINFPC, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -1658,10 +1937,12 @@
           <t>(GIINFIP2, Aprobada)</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1694,10 +1975,20 @@
           <t>(GIINDTE1, Aprobada)</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>(GIINDDOSIG, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>(GIINDDOSIG, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>89</v>
+        <v>35</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1730,10 +2021,12 @@
           <t>(GIINDAL2, Aprobada), (GIINDEST2, Aprobada)</t>
         </is>
       </c>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -1766,10 +2059,20 @@
           <t>(GIINFDS, Aprobada)</t>
         </is>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>(GIINFDDP, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>(GIINFDDP, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -1802,10 +2105,20 @@
           <t>(GIINFSISOP, Aprobada), (GIINFLP, Aprobada)</t>
         </is>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>(GIINFSISTD1, Regularizada), (GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>(GIINFSISTD1, Aprobada), (GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1838,10 +2151,20 @@
           <t>(GIINFINGS, Aprobada)</t>
         </is>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1874,10 +2197,20 @@
           <t>(GIINFSISOP, Aprobada), (GIINFRCDA, Aprobada)</t>
         </is>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -1910,10 +2243,20 @@
           <t>(GIINDETGEN, Aprobada)</t>
         </is>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -1946,10 +2289,20 @@
           <t>(GIINFBD, Aprobada), (GIINDEST2, Aprobada)</t>
         </is>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Regularizada)</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1982,10 +2335,12 @@
           <t>(GIINFBD, Aprobada), (GIINFPC, Aprobada)</t>
         </is>
       </c>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>75</v>
+        <v>43</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -2018,10 +2373,12 @@
           <t>(GIINFTE, Aprobada)</t>
         </is>
       </c>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -2054,10 +2411,12 @@
           <t>(GIINFTE, Aprobada)</t>
         </is>
       </c>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -2090,10 +2449,12 @@
           <t>(GIINDTE2, Aprobada)</t>
         </is>
       </c>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -2126,10 +2487,12 @@
           <t>(GIINFPC, Regularizada), (GIINFASCS, Regularizada), (GIINFSEGI, Regularizada), (GIINDETPROF, Regularizada), (GIINFOPMLINF, Regularizada), (GEXTING, Aprobada), (1, Aprobado), (2, Aprobado), (3, Aprobado)</t>
         </is>
       </c>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -2162,10 +2525,20 @@
           <t>(GIINFINGS, Aprobada), (GIINFL3, Aprobada)</t>
         </is>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>(GIINFL4, Regularizada)</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>(GIINFL4, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -2198,10 +2571,12 @@
           <t>(GIINFTE, Aprobada)</t>
         </is>
       </c>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -2234,10 +2609,12 @@
           <t>(GIINFDDP, Aprobada)</t>
         </is>
       </c>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -2270,10 +2647,12 @@
           <t>(GIINFTE, Aprobada)</t>
         </is>
       </c>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -2306,10 +2685,12 @@
           <t>(GIINFTE, Aprobada)</t>
         </is>
       </c>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -2342,10 +2723,12 @@
           <t>(GIINFTE, Aprobada)</t>
         </is>
       </c>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2378,10 +2761,12 @@
           <t>(GIINFTE, Aprobada)</t>
         </is>
       </c>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2406,10 +2791,12 @@
       </c>
       <c r="G56" t="inlineStr"/>
       <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2434,10 +2821,12 @@
       </c>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2462,10 +2851,12 @@
       </c>
       <c r="G58" t="inlineStr"/>
       <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2490,10 +2881,12 @@
       </c>
       <c r="G59" t="inlineStr"/>
       <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -2518,10 +2911,12 @@
       </c>
       <c r="G60" t="inlineStr"/>
       <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -2546,10 +2941,12 @@
       </c>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -2574,10 +2971,12 @@
       </c>
       <c r="G62" t="inlineStr"/>
       <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -2602,10 +3001,12 @@
       </c>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -2630,10 +3031,12 @@
       </c>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -2658,10 +3061,12 @@
       </c>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" s="1" t="n">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -2686,10 +3091,12 @@
       </c>
       <c r="G66" t="inlineStr"/>
       <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -2714,10 +3121,12 @@
       </c>
       <c r="G67" t="inlineStr"/>
       <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -2742,10 +3151,12 @@
       </c>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" s="1" t="n">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -2770,10 +3181,12 @@
       </c>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -2798,10 +3211,12 @@
       </c>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" s="1" t="n">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -2826,10 +3241,12 @@
       </c>
       <c r="G71" t="inlineStr"/>
       <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -2854,10 +3271,12 @@
       </c>
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -2882,10 +3301,12 @@
       </c>
       <c r="G73" t="inlineStr"/>
       <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -2910,10 +3331,12 @@
       </c>
       <c r="G74" t="inlineStr"/>
       <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -2938,10 +3361,12 @@
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" s="1" t="n">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -2966,10 +3391,12 @@
       </c>
       <c r="G76" t="inlineStr"/>
       <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -2994,10 +3421,12 @@
       </c>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -3022,10 +3451,12 @@
       </c>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" s="1" t="n">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -3050,10 +3481,12 @@
       </c>
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -3078,10 +3511,12 @@
       </c>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -3106,10 +3541,12 @@
       </c>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -3134,10 +3571,12 @@
       </c>
       <c r="G82" t="inlineStr"/>
       <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" s="1" t="n">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -3162,10 +3601,12 @@
       </c>
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -3198,10 +3639,12 @@
           <t>(1, Aprobado), (2, Aprobado), (3, Aprobado)</t>
         </is>
       </c>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" s="1" t="n">
-        <v>6</v>
+        <v>83</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -3226,10 +3669,12 @@
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
-        <v>8</v>
+        <v>84</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -3254,10 +3699,12 @@
       </c>
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -3278,10 +3725,20 @@
       <c r="F87" t="inlineStr"/>
       <c r="G87" t="inlineStr"/>
       <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>(GIINFL3, Aprobada), (GIINFPC, Aprobada), (GIINFASCS, Aprobada), (GIINFSEGI, Aprobada), (GIINDETPROF, Aprobada), (GIINFOPMLINF, Aprobada), (GIINFSISTD1, Aprobada), (GIINDTECOM, Aprobada), (GIINDLEG, Aprobada), (GIINDDOSIG, Aprobada), (GIINFTRGRAD, Aprobada), (GIINFDDP, Aprobada), (GIINDCON.Y PRE, Aprobada), (GIINFL4, Aprobada), (GIINDFHUM, Aprobada), (GIINDECON.POL, Aprobada)</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>(GIINFTRGRAD, Aprobada)</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="1" t="n">
-        <v>12</v>
+        <v>86</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -3302,10 +3759,12 @@
       <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" s="1" t="n">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -3330,6 +3789,8 @@
       </c>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
The courses the hovered course is a prerequisite for are now highlighted
</commit_message>
<xml_diff>
--- a/src/data/plan.xlsx
+++ b/src/data/plan.xlsx
@@ -471,12 +471,12 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>is Prerequisite to Take of</t>
+          <t>Prerequisite to Take for</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>is Prerequisite to Pass of</t>
+          <t>Prerequisite to Pass for</t>
         </is>
       </c>
     </row>

</xml_diff>